<commit_message>
update to generate the latest CDS 5.0.3 data
</commit_message>
<xml_diff>
--- a/cds_configuration_files_5.0.0/cds-synthetic_data_values.xlsx
+++ b/cds_configuration_files_5.0.0/cds-synthetic_data_values.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
   <si>
     <t/>
   </si>
@@ -75,7 +75,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -497,7 +497,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -607,7 +609,9 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1253,7 +1257,7 @@
       <c r="DA7" s="2"/>
       <c r="DB7" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1361,7 +1365,7 @@
       <c r="DA8" s="2"/>
       <c r="DB8" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1469,7 +1473,7 @@
       <c r="DA9" s="2"/>
       <c r="DB9" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1577,7 +1581,7 @@
       <c r="DA10" s="2"/>
       <c r="DB10" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1685,7 +1689,7 @@
       <c r="DA11" s="2"/>
       <c r="DB11" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1793,7 +1797,7 @@
       <c r="DA12" s="2"/>
       <c r="DB12" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1901,7 +1905,7 @@
       <c r="DA13" s="2"/>
       <c r="DB13" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2009,7 +2013,7 @@
       <c r="DA14" s="2"/>
       <c r="DB14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2117,7 +2121,7 @@
       <c r="DA15" s="2"/>
       <c r="DB15" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2225,7 +2229,7 @@
       <c r="DA16" s="2"/>
       <c r="DB16" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -2333,7 +2337,7 @@
       <c r="DA17" s="2"/>
       <c r="DB17" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>

</xml_diff>